<commit_message>
python fertig aber muss zugeordnet werden
</commit_message>
<xml_diff>
--- a/v5/Messwerte v5.xlsx
+++ b/v5/Messwerte v5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds-05\Desktop\v5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds-05\Desktop\SSS\v5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>v2</t>
   </si>
@@ -42,14 +42,37 @@
   </si>
   <si>
     <t>Oszil</t>
+  </si>
+  <si>
+    <t>ei AD</t>
+  </si>
+  <si>
+    <t>ei Phil</t>
+  </si>
+  <si>
+    <t>Quanfehler</t>
+  </si>
+  <si>
+    <t>standardabweichung</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>Samplerate</t>
+  </si>
+  <si>
+    <t>8021.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.000000000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -80,10 +103,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -364,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,12 +400,12 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -390,8 +415,17 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -404,8 +438,20 @@
       <c r="E3">
         <v>1.0389999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <f>E3-C3</f>
+        <v>3.8437499999999236E-3</v>
+      </c>
+      <c r="G3">
+        <f>E3-D3</f>
+        <v>-5.1000000000000156E-2</v>
+      </c>
+      <c r="I3">
+        <f>20/2^11</f>
+        <v>9.765625E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -418,8 +464,16 @@
       <c r="E4">
         <v>2.0009999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F12" si="0">E4-C4</f>
+        <v>8.8124999999998899E-3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G12" si="1">E4-D4</f>
+        <v>9.9999999999988987E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -432,8 +486,16 @@
       <c r="E5">
         <v>3.06</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>5.2187500000000053E-2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -446,8 +508,16 @@
       <c r="E6">
         <v>4.07</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>7.5000000000002842E-3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-1.9999999999999574E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -460,8 +530,16 @@
       <c r="E7">
         <v>5.0819999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8749999999998508E-3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>-8.0000000000000071E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -474,8 +552,16 @@
       <c r="E8">
         <v>5.9980000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>1.167187500000022E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>-5.1999999999999602E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
@@ -488,8 +574,16 @@
       <c r="E9">
         <v>7.01</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>-4.0781250000000213E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>-4.9999999999999822E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
@@ -502,8 +596,16 @@
       <c r="E10">
         <v>8.0220000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>-4.4406249999999758E-2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>-5.7999999999999829E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
@@ -516,8 +618,16 @@
       <c r="E11">
         <v>8.9860000000000007</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.6031249999999346E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-0.1039999999999992</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -530,117 +640,198 @@
       <c r="E12">
         <v>9.9990000000000006</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8531250000000554E-2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.30900000000000105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3">
+        <f>SQRT(SUMSQ(F3:F12)/9)</f>
+        <v>4.2457693467639085E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <f>SQRT(SUMSQ(G3:G12)/9)</f>
+        <v>0.11466424416045716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>0.5</v>
       </c>
       <c r="D15">
         <v>0.51900000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <f>C15-D15</f>
+        <v>-1.9000000000000017E-2</v>
+      </c>
+      <c r="I15">
+        <f>5/2^10</f>
+        <v>4.8828125E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4">
+        <f t="shared" ref="E16:E24" si="2">C16-D16</f>
+        <v>-8.0000000000000071E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>1.5</v>
       </c>
       <c r="D17" s="1">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.12000000000000011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>2.5</v>
       </c>
       <c r="D19">
         <v>2.63</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.12999999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>3</v>
       </c>
       <c r="D20">
         <v>3.13</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.12999999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>3.5</v>
       </c>
       <c r="D21" s="1">
         <v>3.67</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.16999999999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>4</v>
       </c>
       <c r="D22">
         <v>4.18</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.17999999999999972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>4.5</v>
       </c>
       <c r="D23">
         <v>4.6900000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.19000000000000039</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>5</v>
       </c>
       <c r="D24">
         <v>5.17</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.16999999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="3">
+        <f>SQRT(SUMSQ(E15:E24)/9)</f>
+        <v>0.14577798949849124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>